<commit_message>
neue methode: zauber wirken
</commit_message>
<xml_diff>
--- a/data/zauber.xlsx
+++ b/data/zauber.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRH\Documents\GitHub\srh_proj_dsa\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaelm\srh_proj_dsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EA943C-CF52-4EE3-956C-16CE389E2A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6DB62C-7310-4BE3-A13C-F15623E8B5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Zauber</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Eigenschaftsprobe</t>
   </si>
   <si>
-    <t>Dauer</t>
-  </si>
-  <si>
     <t>Kosten</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>MU/IN/CH</t>
   </si>
   <si>
-    <t>4 Aktionen</t>
-  </si>
-  <si>
     <t>8 AsP</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>MU/KL/CH</t>
   </si>
   <si>
-    <t>1 Aktion</t>
-  </si>
-  <si>
     <t>8 Schritt</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>Ignifaxius</t>
   </si>
   <si>
-    <t>2 Aktionen</t>
-  </si>
-  <si>
     <t>16 Schritt</t>
   </si>
   <si>
@@ -93,13 +81,37 @@
     <t>1 AsP</t>
   </si>
   <si>
-    <t>2 Asp</t>
-  </si>
-  <si>
     <t>pro Stunde</t>
   </si>
   <si>
     <t>0 AsP</t>
+  </si>
+  <si>
+    <t>Schaden</t>
+  </si>
+  <si>
+    <t>2 w6</t>
+  </si>
+  <si>
+    <t>QS</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>Zauberdauer</t>
+  </si>
+  <si>
+    <t>4 Aktion(en)</t>
+  </si>
+  <si>
+    <t>1 Aktion(en)</t>
+  </si>
+  <si>
+    <t>2 Aktion(en)</t>
+  </si>
+  <si>
+    <t>2 AsP</t>
   </si>
 </sst>
 </file>
@@ -420,24 +432,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="27.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.88671875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="24" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="27.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,88 +455,112 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>